<commit_message>
added method to run analysis from json
I tested this with an analysis made from a sample spreadsheet (also
included in this commit). Next I need to extend the ruby generated
analysis json to have all of the necessary objects for a multi-datapiont
run.
</commit_message>
<xml_diff>
--- a/projects/workflow_option_a_test.xlsx
+++ b/projects/workflow_option_a_test.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="779">
   <si>
     <t>type</t>
   </si>
@@ -4143,9 +4143,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -4161,6 +4158,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1503">
@@ -5968,7 +5968,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6261,9 +6261,8 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-2))=0,"",INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-2))</f>
         <v>Sample Method</v>
       </c>
-      <c r="B25" s="18" t="str">
-        <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-1))=0,"",INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-1)))</f>
-        <v>individual_variables</v>
+      <c r="B25" s="18" t="s">
+        <v>453</v>
       </c>
       <c r="C25" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))=0,"",INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))</f>
@@ -6278,15 +6277,13 @@
         <v>Number of Samples</v>
       </c>
       <c r="B26" s="18">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="C26" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AF$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))=0,"",INDEX(Lookups!$C$19:$AF$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
-      <c r="D26" s="27">
-        <v>20</v>
-      </c>
+      <c r="D26" s="27"/>
       <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -6496,25 +6493,25 @@
         <v>698</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="48" t="s">
+    <row r="41" spans="1:6" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="51" t="s">
         <v>777</v>
       </c>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-    </row>
-    <row r="42" spans="1:6" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="48" t="s">
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+    </row>
+    <row r="42" spans="1:6" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="51" t="s">
         <v>778</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
@@ -6699,14 +6696,14 @@
       <c r="R1" s="33"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
@@ -7252,43 +7249,43 @@
       <c r="Y14" s="42"/>
       <c r="Z14" s="42"/>
     </row>
-    <row r="15" spans="1:26" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47" t="s">
+    <row r="15" spans="1:26" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46" t="s">
         <v>748</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47" t="s">
+      <c r="F15" s="46"/>
+      <c r="G15" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47">
-        <v>2</v>
-      </c>
-      <c r="J15" s="47"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="47"/>
-      <c r="S15" s="47"/>
-      <c r="T15" s="47"/>
-      <c r="U15" s="47"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="47"/>
-      <c r="X15" s="47"/>
-      <c r="Y15" s="47"/>
-      <c r="Z15" s="47"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46">
+        <v>2</v>
+      </c>
+      <c r="J15" s="46"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
+      <c r="Z15" s="46"/>
     </row>
     <row r="16" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
@@ -7322,7 +7319,7 @@
       <c r="M16" s="43">
         <v>10</v>
       </c>
-      <c r="N16" s="53">
+      <c r="N16" s="52">
         <v>3</v>
       </c>
       <c r="O16" s="43"/>
@@ -7408,7 +7405,7 @@
       <c r="M18" s="43">
         <v>0.4</v>
       </c>
-      <c r="N18" s="53">
+      <c r="N18" s="52">
         <v>0.5</v>
       </c>
       <c r="O18" s="43"/>
@@ -7486,7 +7483,7 @@
       <c r="I20" s="15" t="s">
         <v>760</v>
       </c>
-      <c r="J20" s="50" t="s">
+      <c r="J20" s="49" t="s">
         <v>83</v>
       </c>
       <c r="K20" s="41"/>
@@ -7574,7 +7571,7 @@
       <c r="M22" s="43">
         <v>0.4</v>
       </c>
-      <c r="N22" s="53">
+      <c r="N22" s="52">
         <v>0.5</v>
       </c>
       <c r="O22" s="43"/>
@@ -7645,14 +7642,14 @@
         <v>80</v>
       </c>
       <c r="F24" s="15"/>
-      <c r="G24" s="51" t="s">
+      <c r="G24" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51" t="s">
+      <c r="H24" s="50"/>
+      <c r="I24" s="50" t="s">
         <v>653</v>
       </c>
-      <c r="J24" s="50" t="s">
+      <c r="J24" s="49" t="s">
         <v>83</v>
       </c>
       <c r="K24" s="41"/>
@@ -7740,7 +7737,7 @@
       <c r="M26" s="43">
         <v>0.4</v>
       </c>
-      <c r="N26" s="53">
+      <c r="N26" s="52">
         <v>0.5</v>
       </c>
       <c r="O26" s="43"/>
@@ -7811,14 +7808,14 @@
         <v>80</v>
       </c>
       <c r="F28" s="15"/>
-      <c r="G28" s="51" t="s">
+      <c r="G28" s="50" t="s">
         <v>61</v>
       </c>
       <c r="H28" s="15"/>
       <c r="I28" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="49" t="s">
         <v>83</v>
       </c>
       <c r="K28" s="41"/>
@@ -7906,7 +7903,7 @@
       <c r="M30" s="43">
         <v>0.4</v>
       </c>
-      <c r="N30" s="53">
+      <c r="N30" s="52">
         <v>0.5</v>
       </c>
       <c r="O30" s="43"/>
@@ -7977,14 +7974,14 @@
         <v>80</v>
       </c>
       <c r="F32" s="15"/>
-      <c r="G32" s="51" t="s">
+      <c r="G32" s="50" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="15"/>
       <c r="I32" s="15" t="s">
         <v>611</v>
       </c>
-      <c r="J32" s="50" t="s">
+      <c r="J32" s="49" t="s">
         <v>83</v>
       </c>
       <c r="K32" s="41"/>
@@ -8245,7 +8242,7 @@
         <v>773</v>
       </c>
       <c r="F39" s="15"/>
-      <c r="G39" s="51" t="s">
+      <c r="G39" s="50" t="s">
         <v>103</v>
       </c>
       <c r="H39" s="15"/>

</xml_diff>

<commit_message>
test work multi datapoint workflow a running
Next I need to add output objective functions and add input for analysis
characteristics to the workflow script vs. hard coded in run.rake
</commit_message>
<xml_diff>
--- a/projects/workflow_option_a_test.xlsx
+++ b/projects/workflow_option_a_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="8085" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="8085" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="780">
   <si>
     <t>type</t>
   </si>
@@ -2372,6 +2372,9 @@
   </si>
   <si>
     <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.stat</t>
+  </si>
+  <si>
+    <t>Set Building Defaults</t>
   </si>
 </sst>
 </file>
@@ -5967,8 +5970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6639,8 +6642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7015,8 +7018,8 @@
         <v>21</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
-        <v>58</v>
+      <c r="D9" s="50" t="s">
+        <v>779</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>740</v>

</xml_diff>